<commit_message>
uploading the raw files of budget at a glance
</commit_message>
<xml_diff>
--- a/projects/union-budget/data/raw/union-budget-2020-2021.xlsx
+++ b/projects/union-budget/data/raw/union-budget-2020-2021.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <r>
       <t xml:space="preserve">2018-2019
@@ -240,6 +240,21 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">14. राजस्व घाटा </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="9"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(10-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve"> 14. Revenue Deficit </t>
     </r>
     <r>
@@ -363,6 +378,22 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">15. प्रभावी राजस्व घाटा 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">     (14-12)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve"> 15. Effective Revenue Deficit
 </t>
     </r>
@@ -507,6 +538,22 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">16. राजकोषीय घाटा
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">      [9-(1+5+6)]</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve"> 16. Fiscal Deficit 
 </t>
     </r>
@@ -641,6 +688,21 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">17. प्राथमिक घाटा </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="9"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(16-11)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve"> 17. Primary Deficit </t>
     </r>
     <r>
@@ -761,6 +823,57 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> बजट का सार Budget at a Glance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (₹ करोड़) (In ₹ crores)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. राजस्व प्राप्तियां </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2. कर राजस्व (केंद्र को निवल )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3. कर भिन्न राजस्व </t>
+  </si>
+  <si>
+    <t>4. पूंजी प्राप्तियां ¹</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5. ऋणों की वसूली </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6. अन्य  प्राप्तियां </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7. उधार और अन्य देयताएं²</t>
+  </si>
+  <si>
+    <t>8. कुल प्राप्तियां (1+4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. कुल व्यय (10+13) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    10. राजस्व  खाते पर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         जिसमें से </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    11. ब्याज भुगतान </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    12. पूंजी परिसंपत्तियों के सृजन</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         हेतु सहायता अनुदान</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    13. पूंजी खाते पर </t>
   </si>
   <si>
     <t>499544
@@ -777,6 +890,163 @@
   <si>
     <t>141741
 (0.7)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1 इससे नगदी शेष में आहरण द्वारा कमी शामिल है 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">टिप्पणी :
+             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>(i) 2019-2020</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> के संशोधित अनुमान में </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.5"/>
+        <color indexed="11"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">20442233 करोड़  के अनुमानित सघउ की तुलना में 10.0 % की वृद्धि दर मानते हुए 2020-2021 के बजट 
+                  अनुमान में सघउ बढ़कर </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.5"/>
+        <color indexed="11"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>₹  22489420</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8.5"/>
+        <color indexed="11"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">करोड़ होने का पूर्वानुमान है 
+             (ii) इस दस्तावेज, पृथक -पृथक मदें पूर्णकन के कारण संभवतः जोड़ से मेल न खाएं  
+             (iii) कोष्ठक में दियें गए आंकड़े सघउ के प्रतिशत के रूप में है 
+1  Includes drawdown of cash Balance
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Notes:
+           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (i) GDP for BE 2020-2021  has been projected at  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="11"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>₹  22489420</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> crore assuming 10.0 % growth over the estimated GDP 
+                  of  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="11"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">₹ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Nirmala UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>20442233 crore for 2019-2020(RE).
+            (ii) Individual items in this document may not sum up to the totals due to rounding off
+            (iii) Figures in parenthesis are as a percentage of GDP</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -786,10 +1056,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-10409]0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="15"/>
+      <color indexed="9"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8.5"/>
+      <color indexed="11"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -860,6 +1145,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color indexed="11"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="11"/>
+      <name val="Nirmala UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -901,25 +1211,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -935,19 +1233,43 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1324,411 +1646,487 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="B1:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B27" sqref="B27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="2:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="D4" s="4">
         <v>1552916</v>
       </c>
-      <c r="C2" s="5">
+      <c r="E4" s="5">
         <v>1962761</v>
       </c>
-      <c r="D2" s="4">
+      <c r="F4" s="4">
         <v>1850101</v>
       </c>
-      <c r="E2" s="4">
+      <c r="G4" s="4">
         <v>2020926</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="D5" s="7">
         <v>1317211</v>
       </c>
-      <c r="C3" s="8">
+      <c r="E5" s="8">
         <v>1649582</v>
       </c>
-      <c r="D3" s="7">
+      <c r="F5" s="7">
         <v>1504587</v>
       </c>
-      <c r="E3" s="7">
+      <c r="G5" s="7">
         <v>1635909</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="D6" s="7">
         <v>235705</v>
       </c>
-      <c r="C4" s="8">
+      <c r="E6" s="8">
         <v>313179</v>
       </c>
-      <c r="D4" s="7">
+      <c r="F6" s="7">
         <v>345514</v>
       </c>
-      <c r="E4" s="7">
+      <c r="G6" s="7">
         <v>385017</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="D8" s="4">
         <v>762197</v>
       </c>
-      <c r="C6" s="5">
+      <c r="E8" s="5">
         <v>823588</v>
       </c>
-      <c r="D6" s="4">
+      <c r="F8" s="4">
         <v>848451</v>
       </c>
-      <c r="E6" s="4">
+      <c r="G8" s="4">
         <v>1021304</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
+      <c r="D9" s="7">
         <v>18052</v>
       </c>
-      <c r="C7" s="8">
+      <c r="E9" s="8">
         <v>14828</v>
       </c>
-      <c r="D7" s="7">
+      <c r="F9" s="7">
         <v>16605</v>
       </c>
-      <c r="E7" s="7">
+      <c r="G9" s="7">
         <v>14967</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="10" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7">
+      <c r="D10" s="7">
         <v>94727</v>
       </c>
-      <c r="C8" s="8">
+      <c r="E10" s="8">
         <v>105000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="F10" s="7">
         <v>65000</v>
       </c>
-      <c r="E8" s="7">
+      <c r="G10" s="7">
         <v>210000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="D11" s="7">
         <v>649418</v>
       </c>
-      <c r="C9" s="8">
+      <c r="E11" s="8">
         <v>703760</v>
       </c>
-      <c r="D9" s="7">
+      <c r="F11" s="7">
         <v>766846</v>
       </c>
-      <c r="E9" s="7">
+      <c r="G11" s="7">
         <v>796337</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="12" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2315113</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2786349</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2698552</v>
-      </c>
-      <c r="E11" s="4">
-        <v>3042230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2315113</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2786349</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2698552</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3042230</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="D15" s="4">
         <v>2315113</v>
       </c>
-      <c r="C13" s="5">
+      <c r="E15" s="5">
         <v>2786349</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F15" s="4">
         <v>2698552</v>
       </c>
-      <c r="E13" s="4">
+      <c r="G15" s="4">
         <v>3042230</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="16" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7">
+      <c r="D16" s="7">
         <v>2007399</v>
       </c>
-      <c r="C14" s="8">
+      <c r="E16" s="8">
         <v>2447780</v>
       </c>
-      <c r="D14" s="7">
+      <c r="F16" s="7">
         <v>2349645</v>
       </c>
-      <c r="E14" s="7">
+      <c r="G16" s="7">
         <v>2630145</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="17" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="7">
+      <c r="D18" s="7">
         <v>582648</v>
       </c>
-      <c r="C16" s="8">
+      <c r="E18" s="8">
         <v>660471</v>
       </c>
-      <c r="D16" s="7">
+      <c r="F18" s="7">
         <v>625105</v>
       </c>
-      <c r="E16" s="7">
+      <c r="G18" s="7">
         <v>708203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7">
+      <c r="D19" s="7">
         <v>191781</v>
       </c>
-      <c r="C17" s="8">
+      <c r="E19" s="8">
         <v>207333</v>
       </c>
-      <c r="D17" s="7">
+      <c r="F19" s="7">
         <v>191737</v>
       </c>
-      <c r="E17" s="7">
+      <c r="G19" s="7">
         <v>206500</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="20" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="7">
-        <v>307714</v>
-      </c>
-      <c r="C19" s="8">
-        <v>338569</v>
-      </c>
-      <c r="D19" s="7">
-        <v>348907</v>
-      </c>
-      <c r="E19" s="7">
-        <v>412085</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="7">
+        <v>307714</v>
+      </c>
+      <c r="E21" s="8">
+        <v>338569</v>
+      </c>
+      <c r="F21" s="7">
+        <v>348907</v>
+      </c>
+      <c r="G21" s="7">
+        <v>412085</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="D26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="E26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="F26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+    </row>
+    <row r="27" spans="2:7" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A28:E28"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B27:G27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="0.5" bottom="0.53" header="0.5" footer="0.5"/>

</xml_diff>